<commit_message>
update excel upload api
</commit_message>
<xml_diff>
--- a/reverb-sample.xlsx
+++ b/reverb-sample.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="111">
   <si>
     <t>Artist Name</t>
   </si>
@@ -288,6 +288,90 @@
   </si>
   <si>
     <t>Rishabh Agrawal/Mayank Mittal</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>artist-1.jpg</t>
+  </si>
+  <si>
+    <t>artist-2.jpg</t>
+  </si>
+  <si>
+    <t>artist-3.jpg</t>
+  </si>
+  <si>
+    <t>artist-27.jpg</t>
+  </si>
+  <si>
+    <t>artist-26.jpg</t>
+  </si>
+  <si>
+    <t>artist-24.jpg</t>
+  </si>
+  <si>
+    <t>artist-23.jpg</t>
+  </si>
+  <si>
+    <t>artist-22.jpg</t>
+  </si>
+  <si>
+    <t>artist-21.jpg</t>
+  </si>
+  <si>
+    <t>artist-15.jpg</t>
+  </si>
+  <si>
+    <t>artist-17.jpg</t>
+  </si>
+  <si>
+    <t>artist-18.jpg</t>
+  </si>
+  <si>
+    <t>artist-20.jpg</t>
+  </si>
+  <si>
+    <t>artist-19.jpg</t>
+  </si>
+  <si>
+    <t>artist-12.jpg</t>
+  </si>
+  <si>
+    <t>artist-13.jpg</t>
+  </si>
+  <si>
+    <t>artist-11.jpg</t>
+  </si>
+  <si>
+    <t>artist-10.jpg</t>
+  </si>
+  <si>
+    <t>artist-9.jpg</t>
+  </si>
+  <si>
+    <t>artist-8.jpg</t>
+  </si>
+  <si>
+    <t>artist-7.jpg</t>
+  </si>
+  <si>
+    <t>artist-4.jpg</t>
+  </si>
+  <si>
+    <t>artist-6.jpg,artist-60.jpg</t>
+  </si>
+  <si>
+    <t>artist-16.jpg,artist-59.jpg</t>
+  </si>
+  <si>
+    <t>artist-14.jpg,artist-58.jpg</t>
+  </si>
+  <si>
+    <t>artist-25.jpg,artist-57.jpg</t>
+  </si>
+  <si>
+    <t>artist-5.jpg,artist-62.jpg,artist-61.jpg</t>
   </si>
 </sst>
 </file>
@@ -706,10 +790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N37"/>
+  <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="I26" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -728,9 +812,10 @@
     <col min="12" max="12" width="24.6640625" customWidth="1"/>
     <col min="13" max="13" width="23.6640625" customWidth="1"/>
     <col min="14" max="14" width="16.83203125" customWidth="1"/>
+    <col min="16" max="16" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -773,8 +858,11 @@
       <c r="N1" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="253" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O1" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="253" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>14</v>
       </c>
@@ -811,8 +899,11 @@
       <c r="N2" s="7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" ht="67" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O2" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="67" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>35</v>
       </c>
@@ -843,8 +934,11 @@
       <c r="N3" s="7" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" ht="240" x14ac:dyDescent="0.2">
+      <c r="O3" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="240" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>36</v>
       </c>
@@ -875,8 +969,11 @@
       <c r="N4" s="7" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" ht="240" x14ac:dyDescent="0.2">
+      <c r="O4" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="240" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>37</v>
       </c>
@@ -905,8 +1002,11 @@
       <c r="N5" s="7" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" ht="240" x14ac:dyDescent="0.2">
+      <c r="O5" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="240" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>38</v>
       </c>
@@ -929,8 +1029,11 @@
         <v>65</v>
       </c>
       <c r="N6" s="7"/>
-    </row>
-    <row r="7" spans="1:14" ht="256" x14ac:dyDescent="0.2">
+      <c r="O6" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="256" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>39</v>
       </c>
@@ -957,8 +1060,11 @@
       <c r="N7" s="7" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" ht="176" x14ac:dyDescent="0.2">
+      <c r="O7" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="176" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>40</v>
       </c>
@@ -987,8 +1093,11 @@
       <c r="N8" s="12" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" ht="272" x14ac:dyDescent="0.2">
+      <c r="O8" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="272" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>41</v>
       </c>
@@ -1015,8 +1124,11 @@
       <c r="N9" s="12" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" ht="240" x14ac:dyDescent="0.2">
+      <c r="O9" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="240" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>42</v>
       </c>
@@ -1043,8 +1155,11 @@
       <c r="N10" s="12" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" ht="128" x14ac:dyDescent="0.2">
+      <c r="O10" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="128" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>43</v>
       </c>
@@ -1071,8 +1186,11 @@
       <c r="N11" s="12" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" ht="240" x14ac:dyDescent="0.2">
+      <c r="O11" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="240" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>44</v>
       </c>
@@ -1101,8 +1219,11 @@
       <c r="N12" s="12" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" ht="192" x14ac:dyDescent="0.2">
+      <c r="O12" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="192" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>45</v>
       </c>
@@ -1129,8 +1250,11 @@
       <c r="N13" s="12" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+      <c r="O13" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>46</v>
       </c>
@@ -1155,8 +1279,11 @@
       <c r="N14" s="12" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="O14" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>47</v>
       </c>
@@ -1179,8 +1306,11 @@
       <c r="N15" s="12" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" ht="128" x14ac:dyDescent="0.2">
+      <c r="O15" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="128" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>48</v>
       </c>
@@ -1205,8 +1335,11 @@
       <c r="N16" s="12" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+      <c r="O16" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>49</v>
       </c>
@@ -1233,8 +1366,11 @@
       <c r="N17" s="12" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+      <c r="O17" s="7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>50</v>
       </c>
@@ -1261,8 +1397,11 @@
       <c r="N18" s="4" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+      <c r="O18" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
         <v>51</v>
       </c>
@@ -1287,8 +1426,11 @@
       <c r="N19" s="12" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+      <c r="O19" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
         <v>52</v>
       </c>
@@ -1313,8 +1455,11 @@
       <c r="N20" s="12" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+      <c r="O20" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
         <v>53</v>
       </c>
@@ -1341,8 +1486,11 @@
       <c r="N21" s="12" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+      <c r="O21" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
         <v>54</v>
       </c>
@@ -1369,8 +1517,11 @@
       <c r="N22" s="12" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="O22" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
         <v>55</v>
       </c>
@@ -1393,8 +1544,11 @@
       <c r="N23" s="12" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="O23" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
         <v>56</v>
       </c>
@@ -1427,8 +1581,11 @@
       <c r="N24" s="12" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+      <c r="O24" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
         <v>57</v>
       </c>
@@ -1451,8 +1608,11 @@
       <c r="N25" s="12" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="O25" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
         <v>58</v>
       </c>
@@ -1485,8 +1645,11 @@
       <c r="N26" s="12" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="O26" s="7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
         <v>77</v>
       </c>
@@ -1509,8 +1672,11 @@
       <c r="N27" s="12" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="O27" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
         <v>78</v>
       </c>
@@ -1543,19 +1709,22 @@
       <c r="N28" s="12" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O28" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E29" s="3"/>
       <c r="H29" s="4"/>
       <c r="M29" s="11"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="M30" s="11"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="M31" s="11"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="M32" s="11"/>
     </row>
     <row r="33" spans="13:13" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update artist excel api
</commit_message>
<xml_diff>
--- a/reverb-sample.xlsx
+++ b/reverb-sample.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15920" tabRatio="500"/>
+    <workbookView minimized="1" xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -293,12 +293,6 @@
     <t>Image</t>
   </si>
   <si>
-    <t>artist-1.jpg</t>
-  </si>
-  <si>
-    <t>artist-2.jpg</t>
-  </si>
-  <si>
     <t>artist-3.jpg</t>
   </si>
   <si>
@@ -372,6 +366,12 @@
   </si>
   <si>
     <t>artist-5.jpg,artist-62.jpg,artist-61.jpg</t>
+  </si>
+  <si>
+    <t>artist-1.jpg,artist-5.jpg,artist-62.jpg,artist-61.jpg</t>
+  </si>
+  <si>
+    <t>artist-1.jpg,artist-5.jpg,artist-61.jpg</t>
   </si>
 </sst>
 </file>
@@ -792,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I26" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -900,7 +900,7 @@
         <v>22</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="67" customHeight="1" x14ac:dyDescent="0.2">
@@ -935,7 +935,7 @@
         <v>67</v>
       </c>
       <c r="O3" s="7" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="240" x14ac:dyDescent="0.2">
@@ -970,7 +970,7 @@
         <v>68</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="240" x14ac:dyDescent="0.2">
@@ -1003,7 +1003,7 @@
         <v>68</v>
       </c>
       <c r="O5" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="240" x14ac:dyDescent="0.2">
@@ -1030,7 +1030,7 @@
       </c>
       <c r="N6" s="7"/>
       <c r="O6" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="256" x14ac:dyDescent="0.2">
@@ -1061,7 +1061,7 @@
         <v>69</v>
       </c>
       <c r="O7" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="176" x14ac:dyDescent="0.2">
@@ -1094,7 +1094,7 @@
         <v>72</v>
       </c>
       <c r="O8" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="272" x14ac:dyDescent="0.2">
@@ -1125,7 +1125,7 @@
         <v>73</v>
       </c>
       <c r="O9" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="240" x14ac:dyDescent="0.2">
@@ -1156,7 +1156,7 @@
         <v>72</v>
       </c>
       <c r="O10" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="128" x14ac:dyDescent="0.2">
@@ -1187,7 +1187,7 @@
         <v>73</v>
       </c>
       <c r="O11" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="240" x14ac:dyDescent="0.2">
@@ -1220,7 +1220,7 @@
         <v>72</v>
       </c>
       <c r="O12" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="192" x14ac:dyDescent="0.2">
@@ -1251,7 +1251,7 @@
         <v>72</v>
       </c>
       <c r="O13" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="45" x14ac:dyDescent="0.2">
@@ -1280,7 +1280,7 @@
         <v>72</v>
       </c>
       <c r="O14" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="48" x14ac:dyDescent="0.2">
@@ -1307,7 +1307,7 @@
         <v>74</v>
       </c>
       <c r="O15" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="128" x14ac:dyDescent="0.2">
@@ -1336,7 +1336,7 @@
         <v>72</v>
       </c>
       <c r="O16" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="48" x14ac:dyDescent="0.2">
@@ -1367,7 +1367,7 @@
         <v>75</v>
       </c>
       <c r="O17" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="45" x14ac:dyDescent="0.2">
@@ -1398,7 +1398,7 @@
         <v>76</v>
       </c>
       <c r="O18" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="32" x14ac:dyDescent="0.2">
@@ -1427,7 +1427,7 @@
         <v>72</v>
       </c>
       <c r="O19" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="45" x14ac:dyDescent="0.2">
@@ -1456,7 +1456,7 @@
         <v>72</v>
       </c>
       <c r="O20" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="45" x14ac:dyDescent="0.2">
@@ -1487,7 +1487,7 @@
         <v>72</v>
       </c>
       <c r="O21" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="45" x14ac:dyDescent="0.2">
@@ -1518,7 +1518,7 @@
         <v>72</v>
       </c>
       <c r="O22" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="48" x14ac:dyDescent="0.2">
@@ -1545,7 +1545,7 @@
         <v>72</v>
       </c>
       <c r="O23" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="48" x14ac:dyDescent="0.2">
@@ -1582,7 +1582,7 @@
         <v>74</v>
       </c>
       <c r="O24" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="32" x14ac:dyDescent="0.2">
@@ -1609,7 +1609,7 @@
         <v>72</v>
       </c>
       <c r="O25" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="48" x14ac:dyDescent="0.2">
@@ -1646,7 +1646,7 @@
         <v>75</v>
       </c>
       <c r="O26" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="48" x14ac:dyDescent="0.2">
@@ -1673,7 +1673,7 @@
         <v>72</v>
       </c>
       <c r="O27" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="48" x14ac:dyDescent="0.2">
@@ -1710,7 +1710,7 @@
         <v>74</v>
       </c>
       <c r="O28" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">

</xml_diff>